<commit_message>
updated checklists for mistakes found by nikhil
</commit_message>
<xml_diff>
--- a/nhsrc/kayakalp/Kayakalp-UPHC-APHC-28-July-2016.xlsx
+++ b/nhsrc/kayakalp/Kayakalp-UPHC-APHC-28-July-2016.xlsx
@@ -28,7 +28,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="page207" vbProcedure="false">'kayakalp uphcaphc'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="page209" vbProcedure="false">'kayakalp uphcaphc'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Kayakalp!$A$1:$M$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Kayakalp!$A$1:$M$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Kayakalp!$A$1:$M$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Kayakalp!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Kayakalp!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Kayakalp!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Kayakalp!$A$1:$M$157</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="428">
   <si>
     <t xml:space="preserve">Ref. No.</t>
   </si>
@@ -61,13 +65,10 @@
     <t xml:space="preserve">Remarks</t>
   </si>
   <si>
-    <t xml:space="preserve">A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHC UPKEEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A1</t>
+    <t xml:space="preserve">Area of Concern – A PHC Upkeep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard A1</t>
   </si>
   <si>
     <t xml:space="preserve">Pest &amp; Animal Control</t>
@@ -98,7 +99,7 @@
     <t xml:space="preserve">Check for the evidence at the facility ( Presence of Pests ,Record of Purchase of Pesticides and availability of the rat trap) and interview the staff</t>
   </si>
   <si>
-    <t xml:space="preserve">A2</t>
+    <t xml:space="preserve">Standard A2</t>
   </si>
   <si>
     <t xml:space="preserve">Landscaping &amp; Gardening</t>
@@ -129,7 +130,7 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">A3</t>
+    <t xml:space="preserve">Standard A3</t>
   </si>
   <si>
     <t xml:space="preserve">Maintenance of Open Areas</t>
@@ -153,7 +154,7 @@
     <t xml:space="preserve">Check for water accumulation in open areas because of faulty drainage, leakage from the pipes, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">A4</t>
+    <t xml:space="preserve">Standard A4</t>
   </si>
   <si>
     <t xml:space="preserve">PHC Appearance</t>
@@ -180,7 +181,7 @@
 Check All signage's (directional &amp; departmental) are in local language and follow uniform colour scheme</t>
   </si>
   <si>
-    <t xml:space="preserve">A5</t>
+    <t xml:space="preserve">Standard A5</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructure Maintenance</t>
@@ -205,7 +206,7 @@
     <t xml:space="preserve">Check that there is a proper boundary wall of adequate height without any breach. Wall is painted in uniform colour</t>
   </si>
   <si>
-    <t xml:space="preserve">A6</t>
+    <t xml:space="preserve">Standard A6</t>
   </si>
   <si>
     <t xml:space="preserve">Illumination</t>
@@ -230,7 +231,7 @@
     <t xml:space="preserve">Check that PHC uses energy efficient bulb like CFL or LED for lighting purpose within the PHC Premises</t>
   </si>
   <si>
-    <t xml:space="preserve">A7</t>
+    <t xml:space="preserve">Standard A7</t>
   </si>
   <si>
     <t xml:space="preserve">Maintenance of Furniture &amp; Fixture</t>
@@ -255,7 +256,7 @@
 Trolleys, Stretchers, Wheel Chairs, etc. are well maintained( As applicable)</t>
   </si>
   <si>
-    <t xml:space="preserve">A8</t>
+    <t xml:space="preserve">Standard A8</t>
   </si>
   <si>
     <t xml:space="preserve">Removal of Junk Material</t>
@@ -279,7 +280,7 @@
     <t xml:space="preserve">Check for availability of a demarcated &amp; secured space for collecting and storing the junk material before its disposal</t>
   </si>
   <si>
-    <t xml:space="preserve">A9</t>
+    <t xml:space="preserve">Standard A9</t>
   </si>
   <si>
     <t xml:space="preserve">Water Conservation</t>
@@ -307,7 +308,7 @@
     <t xml:space="preserve">Check for its functionality and storage system</t>
   </si>
   <si>
-    <t xml:space="preserve">A10</t>
+    <t xml:space="preserve">Standard A10</t>
   </si>
   <si>
     <t xml:space="preserve">Work Place Management</t>
@@ -333,13 +334,10 @@
 Check that drugs, instruments, records, etc. are labelled for facilitating easy identification.</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanitation &amp; Hygiene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1</t>
+    <t xml:space="preserve">Area of Concern – B Sanitation &amp; Hygiene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard B1</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of Circulation Area (Corridors, Waiting area, Lobby, Stairs)</t>
@@ -364,7 +362,7 @@
     <t xml:space="preserve">Ask cleaning staff about frequency of cleaning in a day.</t>
   </si>
   <si>
-    <t xml:space="preserve">B2</t>
+    <t xml:space="preserve">Standard B2</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of OPD Clinic</t>
@@ -389,7 +387,7 @@
     <t xml:space="preserve">Ask cleaning staff about frequency of cleaning in a day. </t>
   </si>
   <si>
-    <t xml:space="preserve">B3</t>
+    <t xml:space="preserve">Standard B3</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of Procedure Areas(Dressing Room, Immunization, Injection Room, Labour Room (if available))</t>
@@ -414,7 +412,7 @@
     <t xml:space="preserve">Ask cleaning staff about frequency of cleaning in a day and also verify with check-list </t>
   </si>
   <si>
-    <t xml:space="preserve">B4</t>
+    <t xml:space="preserve">Standard B4</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of Lab and Pharmacy</t>
@@ -440,7 +438,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">B5</t>
+    <t xml:space="preserve">Standard B5</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of Auxiliary Areas( Office, Meeting Room, Staff Room, Record Room)</t>
@@ -465,7 +463,7 @@
     <t xml:space="preserve">SI/RR</t>
   </si>
   <si>
-    <t xml:space="preserve">B6</t>
+    <t xml:space="preserve">Standard B6</t>
   </si>
   <si>
     <t xml:space="preserve">Cleanliness of Toilets</t>
@@ -490,7 +488,7 @@
     <t xml:space="preserve">Ask cleaning staff to operate cistern and water taps</t>
   </si>
   <si>
-    <t xml:space="preserve">B7</t>
+    <t xml:space="preserve">Standard B7</t>
   </si>
   <si>
     <t xml:space="preserve">Use of standards materials and Equipment for Cleaning</t>
@@ -519,7 +517,7 @@
     <t xml:space="preserve">Check the availability of mops, brooms, collection buckets etc. as per requirement. </t>
   </si>
   <si>
-    <t xml:space="preserve">B8</t>
+    <t xml:space="preserve">Standard B8</t>
   </si>
   <si>
     <t xml:space="preserve">Use of Standard Methods for Cleaning</t>
@@ -544,7 +542,7 @@
 The mop should move from inner area to outer area of the room. Separate mop is used in the procedure area.</t>
   </si>
   <si>
-    <t xml:space="preserve">B9</t>
+    <t xml:space="preserve">Standard B9</t>
   </si>
   <si>
     <t xml:space="preserve">Monitoring of Cleanliness Activities</t>
@@ -571,7 +569,7 @@
     <t xml:space="preserve">Periodic Monitoring is done by MOIC or another designated staff.</t>
   </si>
   <si>
-    <t xml:space="preserve">B10.</t>
+    <t xml:space="preserve">Standard B10.</t>
   </si>
   <si>
     <t xml:space="preserve">Drainage and Sewage Management</t>
@@ -597,13 +595,10 @@
 All the drains are cleaned once in a week</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
+    <t xml:space="preserve">Area of Concern – C Waste Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard C1</t>
   </si>
   <si>
     <t xml:space="preserve">Segregation of Biomedical Waste</t>
@@ -632,7 +627,7 @@
     <t xml:space="preserve">Ask staff about the segregation protocol (Red bag for re-cyclable, Glassware into Cardboard Box with blue marking, etc.)</t>
   </si>
   <si>
-    <t xml:space="preserve">C2</t>
+    <t xml:space="preserve">Standard C2</t>
   </si>
   <si>
     <t xml:space="preserve">Collection and Transportation of Biomedical Waste</t>
@@ -656,7 +651,7 @@
     <t xml:space="preserve">Check availability of trolley for transportation to collection point.</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
+    <t xml:space="preserve">Standard C3</t>
   </si>
   <si>
     <t xml:space="preserve">Sharp Management</t>
@@ -683,7 +678,7 @@
     <t xml:space="preserve">Check availability of Puncture &amp; leak proof container (White Translucent) at point of use for storing needles, syringes with fixed needles, needles from cutter/burner, scalpel blade, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">C4</t>
+    <t xml:space="preserve">Standard C4</t>
   </si>
   <si>
     <t xml:space="preserve">Storage of Biomedical Waste</t>
@@ -707,7 +702,7 @@
     <t xml:space="preserve">Verify that the waste is being disposed / handed over to CTF within 48 hour of generation. Check the record especially during holidays</t>
   </si>
   <si>
-    <t xml:space="preserve">C5</t>
+    <t xml:space="preserve">Standard C5</t>
   </si>
   <si>
     <t xml:space="preserve">Disposal of Biomedical waste</t>
@@ -735,7 +730,7 @@
 (Autoclaving/ Microwaving/ Hydroclaving followed by shredding or a combination of sterilisation and shredding. Later treated waste is handed over to registered vendors.)</t>
   </si>
   <si>
-    <t xml:space="preserve">C6</t>
+    <t xml:space="preserve">Standard C6</t>
   </si>
   <si>
     <t xml:space="preserve">Management Hazardous Waste</t>
@@ -759,7 +754,7 @@
     <t xml:space="preserve">Hazardous chemicals like Glutaraldehyde, Lab Reagents Should not be drained in sewage untreated</t>
   </si>
   <si>
-    <t xml:space="preserve">C7</t>
+    <t xml:space="preserve">Standard C7</t>
   </si>
   <si>
     <t xml:space="preserve">Solid General Waste Management</t>
@@ -783,7 +778,7 @@
     <t xml:space="preserve">Look for efforts of the health facility in managing General Waste, such as Recycling of paper waste, vermicomposting, waste to energy initiative, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">C8</t>
+    <t xml:space="preserve">Standard C8</t>
   </si>
   <si>
     <t xml:space="preserve">Liquid Waste Management</t>
@@ -810,7 +805,7 @@
     <t xml:space="preserve">Check for the procedure - staff interview and direct observation</t>
   </si>
   <si>
-    <t xml:space="preserve">C9</t>
+    <t xml:space="preserve">Standard C9</t>
   </si>
   <si>
     <t xml:space="preserve">Equipment and Supplies for Bio Medical Waste Management</t>
@@ -835,7 +830,7 @@
     <t xml:space="preserve">At each point of generation of sharp waste</t>
   </si>
   <si>
-    <t xml:space="preserve">C10</t>
+    <t xml:space="preserve">Standard C10</t>
   </si>
   <si>
     <t xml:space="preserve">Statuary Compliances</t>
@@ -866,13 +861,10 @@
 d. Immunisation records of all waste handlers</t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infection Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
+    <t xml:space="preserve">Area of Concern – D Infection Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard D1</t>
   </si>
   <si>
     <t xml:space="preserve">Hand Hygiene</t>
@@ -897,7 +889,7 @@
 Ask facility staff to demonstrate 6 steps of normal hand wash and 5 moments of hand washing</t>
   </si>
   <si>
-    <t xml:space="preserve">D2</t>
+    <t xml:space="preserve">Standard D2</t>
   </si>
   <si>
     <t xml:space="preserve">Personal Protective Equipment (PPE)</t>
@@ -921,7 +913,7 @@
     <t xml:space="preserve">Check, if staff uses mask head caps , Lab coat and aprons as applicable</t>
   </si>
   <si>
-    <t xml:space="preserve">D3</t>
+    <t xml:space="preserve">Standard D3</t>
   </si>
   <si>
     <t xml:space="preserve">Personal Protective Practices</t>
@@ -945,7 +937,7 @@
     <t xml:space="preserve">Check that disposable gloves and mask are not re-used. Reusable Gloves and mask are used after adequate sterilization.</t>
   </si>
   <si>
-    <t xml:space="preserve">D4</t>
+    <t xml:space="preserve">Standard D4</t>
   </si>
   <si>
     <t xml:space="preserve">Decontamination and Cleaning of Instruments</t>
@@ -970,7 +962,7 @@
 Ask staff  when and how they clean the surfaces either by chlorine solution or Disinfectant like carbolic acid</t>
   </si>
   <si>
-    <t xml:space="preserve">D5</t>
+    <t xml:space="preserve">Standard D5</t>
   </si>
   <si>
     <t xml:space="preserve">Disinfection &amp; Sterilization of Instruments</t>
@@ -995,7 +987,7 @@
     <t xml:space="preserve">Check with the staff process about of High Level disinfection using Boiling for 20 minutes with lid on, soaking in 2% Glutaraldehyde/Chlorine solution for 20 minutes.</t>
   </si>
   <si>
-    <t xml:space="preserve">D6</t>
+    <t xml:space="preserve">Standard D6</t>
   </si>
   <si>
     <t xml:space="preserve">Spill Management</t>
@@ -1019,7 +1011,7 @@
     <t xml:space="preserve">Check for display</t>
   </si>
   <si>
-    <t xml:space="preserve">D7</t>
+    <t xml:space="preserve">Standard D7</t>
   </si>
   <si>
     <t xml:space="preserve">Isolation and Barrier Nursing</t>
@@ -1043,7 +1035,7 @@
     <t xml:space="preserve">Ask staff about Standard precautions and how they adhere to it.</t>
   </si>
   <si>
-    <t xml:space="preserve">D8</t>
+    <t xml:space="preserve">Standard D8</t>
   </si>
   <si>
     <t xml:space="preserve">Infection Control Program</t>
@@ -1071,7 +1063,7 @@
 Check for the records and lab investigations of staff</t>
   </si>
   <si>
-    <t xml:space="preserve">D9</t>
+    <t xml:space="preserve">Standard D9</t>
   </si>
   <si>
     <t xml:space="preserve">Hospital Acquired Infection Surveillance</t>
@@ -1096,7 +1088,7 @@
 Check records that notifiable disease have been reported in program such as IDSP and AEFI Surveillance.</t>
   </si>
   <si>
-    <t xml:space="preserve">D10</t>
+    <t xml:space="preserve">Standard D10</t>
   </si>
   <si>
     <t xml:space="preserve">Environment Control</t>
@@ -1120,13 +1112,10 @@
     <t xml:space="preserve">Check staff is aware, adhere and promote respiratory hygiene and cough etiquettes</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUPPORT SERVICES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1</t>
+    <t xml:space="preserve">Area of Concern – E Support Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard E1</t>
   </si>
   <si>
     <t xml:space="preserve">Laundry Services &amp; Linen Management</t>
@@ -1150,7 +1139,7 @@
     <t xml:space="preserve">Check facility has in-house or outsourced arrangements for washing linens at least once in a week.</t>
   </si>
   <si>
-    <t xml:space="preserve">E2</t>
+    <t xml:space="preserve">Standard E2</t>
   </si>
   <si>
     <t xml:space="preserve">Water Sanitation</t>
@@ -1177,7 +1166,7 @@
     <t xml:space="preserve">The PHC should have capacity to store 48 hours water requirement Water tank is cleaned at six monthly interval and records are maintained.</t>
   </si>
   <si>
-    <t xml:space="preserve">E3</t>
+    <t xml:space="preserve">Standard E3</t>
   </si>
   <si>
     <t xml:space="preserve">Pharmacy and Stores</t>
@@ -1209,7 +1198,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">E4</t>
+    <t xml:space="preserve">Standard E4</t>
   </si>
   <si>
     <t xml:space="preserve">Security Services</t>
@@ -1233,7 +1222,7 @@
     <t xml:space="preserve">Departments like OPD, Lab, Administrative office etc. are locked after working hours.</t>
   </si>
   <si>
-    <t xml:space="preserve">E5</t>
+    <t xml:space="preserve">Standard E5</t>
   </si>
   <si>
     <t xml:space="preserve">Outreach Services</t>
@@ -1260,13 +1249,10 @@
     <t xml:space="preserve">Check with medical officers and records of monthly meeting ''swachh bharat abhiyan'' has been followed up during monthly meetings with extension workers like MPW, ASHA, ANM etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hygiene Promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1</t>
+    <t xml:space="preserve">Area of Concern – F Hygiene Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard F1</t>
   </si>
   <si>
     <t xml:space="preserve">Community Monitoring &amp; Patient Participation</t>
@@ -1293,7 +1279,7 @@
     <t xml:space="preserve">Check if there is a feedback system for the patients. Verify the records</t>
   </si>
   <si>
-    <t xml:space="preserve">F2</t>
+    <t xml:space="preserve">Standard F2</t>
   </si>
   <si>
     <t xml:space="preserve">Information Education and Communication</t>
@@ -1317,7 +1303,7 @@
     <t xml:space="preserve">Should be displayed prominently in local language</t>
   </si>
   <si>
-    <t xml:space="preserve">F3</t>
+    <t xml:space="preserve">Standard F3</t>
   </si>
   <si>
     <t xml:space="preserve">Leadership and Team work</t>
@@ -1341,7 +1327,7 @@
     <t xml:space="preserve">Ask different members about their roles and responsibilities</t>
   </si>
   <si>
-    <t xml:space="preserve">F4</t>
+    <t xml:space="preserve">Standard F4</t>
   </si>
   <si>
     <t xml:space="preserve">Training and Capacity Building and Standardization</t>
@@ -1365,7 +1351,7 @@
     <t xml:space="preserve">Check staff are trained at the time of induction and once in every year</t>
   </si>
   <si>
-    <t xml:space="preserve">F5</t>
+    <t xml:space="preserve">Standard F5</t>
   </si>
   <si>
     <t xml:space="preserve">Staff Hygiene and Dress Code</t>
@@ -1542,7 +1528,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1599,18 +1585,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1657,14 +1631,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1765,146 +1731,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>795960</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 3" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="570240" y="8448840"/>
-          <a:ext cx="1547640" cy="331560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228240</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 4" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2929680" y="8434800"/>
-          <a:ext cx="1089360" cy="318960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>54360</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1548000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 8" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5299920" y="8562960"/>
-          <a:ext cx="1493640" cy="157320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O160"/>
+  <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A18" colorId="64" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A151" colorId="64" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B153" activeCellId="0" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.01020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.65816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.5051020408163"/>
     <col collapsed="false" hidden="true" max="12" min="9" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="25.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="24.5051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.48469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1937,11 +1787,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1957,10 +1805,10 @@
     </row>
     <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1979,17 +1827,17 @@
     </row>
     <row r="4" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2009,17 +1857,17 @@
     </row>
     <row r="5" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2036,10 +1884,10 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2058,17 +1906,17 @@
     </row>
     <row r="7" customFormat="false" ht="137.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -2083,17 +1931,17 @@
     </row>
     <row r="8" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -2106,15 +1954,15 @@
       <c r="L8" s="3"/>
       <c r="M8" s="8"/>
       <c r="O8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2133,17 +1981,17 @@
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2158,17 +2006,17 @@
     </row>
     <row r="11" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2183,10 +2031,10 @@
     </row>
     <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2205,17 +2053,17 @@
     </row>
     <row r="13" customFormat="false" ht="122.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2230,17 +2078,17 @@
     </row>
     <row r="14" customFormat="false" ht="129" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2255,10 +2103,10 @@
     </row>
     <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2277,17 +2125,17 @@
     </row>
     <row r="16" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -2302,17 +2150,17 @@
     </row>
     <row r="17" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -2327,10 +2175,10 @@
     </row>
     <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2349,17 +2197,17 @@
     </row>
     <row r="19" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2374,17 +2222,17 @@
     </row>
     <row r="20" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -2399,10 +2247,10 @@
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2421,17 +2269,17 @@
     </row>
     <row r="22" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -2446,20 +2294,20 @@
     </row>
     <row r="23" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="8" t="n">
         <v>1</v>
       </c>
@@ -2471,10 +2319,10 @@
     </row>
     <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2493,20 +2341,20 @@
     </row>
     <row r="25" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="8" t="n">
         <v>1</v>
       </c>
@@ -2514,39 +2362,39 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" s="16" customFormat="true" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="15"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -2565,17 +2413,17 @@
     </row>
     <row r="28" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2590,17 +2438,17 @@
     </row>
     <row r="29" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2615,10 +2463,10 @@
     </row>
     <row r="30" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2637,17 +2485,17 @@
     </row>
     <row r="31" customFormat="false" ht="123" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -2662,17 +2510,17 @@
     </row>
     <row r="32" customFormat="false" ht="141" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -2686,11 +2534,9 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="s">
-        <v>93</v>
-      </c>
+      <c r="A33" s="14"/>
       <c r="B33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2706,10 +2552,10 @@
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2728,17 +2574,17 @@
     </row>
     <row r="35" customFormat="false" ht="109.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2753,17 +2599,17 @@
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2778,16 +2624,16 @@
     </row>
     <row r="37" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="6" t="n">
         <f aca="false">SUM(H38:H39)</f>
         <v>2</v>
@@ -2800,20 +2646,20 @@
     </row>
     <row r="38" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="8" t="n">
         <v>1</v>
       </c>
@@ -2825,20 +2671,20 @@
     </row>
     <row r="39" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="8" t="n">
         <v>1</v>
       </c>
@@ -2850,16 +2696,16 @@
     </row>
     <row r="40" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+        <v>109</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
       <c r="H40" s="6" t="n">
         <f aca="false">SUM(H41:H42)</f>
         <v>2</v>
@@ -2872,20 +2718,20 @@
     </row>
     <row r="41" customFormat="false" ht="125.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="8" t="n">
         <v>1</v>
       </c>
@@ -2896,21 +2742,21 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
       <c r="H42" s="8" t="n">
         <v>1</v>
       </c>
@@ -2922,10 +2768,10 @@
     </row>
     <row r="43" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -2944,20 +2790,20 @@
     </row>
     <row r="44" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="8" t="n">
         <v>1</v>
       </c>
@@ -2969,17 +2815,17 @@
     </row>
     <row r="45" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2994,10 +2840,10 @@
     </row>
     <row r="46" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -3016,17 +2862,17 @@
     </row>
     <row r="47" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3041,17 +2887,17 @@
     </row>
     <row r="48" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3066,10 +2912,10 @@
     </row>
     <row r="49" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -3088,17 +2934,17 @@
     </row>
     <row r="50" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -3113,17 +2959,17 @@
     </row>
     <row r="51" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -3138,10 +2984,10 @@
     </row>
     <row r="52" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -3160,17 +3006,17 @@
     </row>
     <row r="53" customFormat="false" ht="169.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -3185,17 +3031,17 @@
     </row>
     <row r="54" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -3210,10 +3056,10 @@
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -3232,17 +3078,17 @@
     </row>
     <row r="56" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -3257,17 +3103,17 @@
     </row>
     <row r="57" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -3282,10 +3128,10 @@
     </row>
     <row r="58" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -3304,17 +3150,17 @@
     </row>
     <row r="59" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -3329,17 +3175,17 @@
     </row>
     <row r="60" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -3354,10 +3200,10 @@
     </row>
     <row r="61" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -3374,44 +3220,44 @@
       <c r="L61" s="3"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" s="16" customFormat="true" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
+    <row r="62" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="15"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -3425,11 +3271,9 @@
       <c r="M63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="19" t="s">
-        <v>177</v>
-      </c>
+      <c r="A64" s="16"/>
       <c r="B64" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3445,10 +3289,10 @@
     </row>
     <row r="65" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -3465,44 +3309,44 @@
       <c r="L65" s="3"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" s="16" customFormat="true" ht="109.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="15"/>
+    <row r="66" customFormat="false" ht="109.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -3517,10 +3361,10 @@
     </row>
     <row r="68" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -3551,17 +3395,17 @@
     </row>
     <row r="69" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -3576,17 +3420,17 @@
     </row>
     <row r="70" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -3601,10 +3445,10 @@
     </row>
     <row r="71" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -3623,17 +3467,17 @@
     </row>
     <row r="72" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -3648,17 +3492,17 @@
     </row>
     <row r="73" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -3671,69 +3515,69 @@
       <c r="L73" s="3"/>
       <c r="M73" s="8"/>
     </row>
-    <row r="74" s="24" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="20"/>
-      <c r="H74" s="21" t="n">
+    <row r="74" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="18" t="n">
         <f aca="false">SUM(H75:H76)</f>
         <v>2</v>
       </c>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="22"/>
-      <c r="L74" s="22"/>
-      <c r="M74" s="23"/>
-    </row>
-    <row r="75" s="16" customFormat="true" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="15"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="19"/>
+      <c r="M74" s="20"/>
+    </row>
+    <row r="75" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
+        <v>132</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
       <c r="H76" s="8" t="n">
         <v>1</v>
       </c>
@@ -3745,10 +3589,10 @@
     </row>
     <row r="77" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -3767,17 +3611,17 @@
     </row>
     <row r="78" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -3792,17 +3636,17 @@
     </row>
     <row r="79" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -3817,10 +3661,10 @@
     </row>
     <row r="80" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -3839,17 +3683,17 @@
     </row>
     <row r="81" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -3864,17 +3708,17 @@
     </row>
     <row r="82" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -3889,10 +3733,10 @@
     </row>
     <row r="83" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -3911,17 +3755,17 @@
     </row>
     <row r="84" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -3936,17 +3780,17 @@
     </row>
     <row r="85" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -3961,10 +3805,10 @@
     </row>
     <row r="86" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -3983,17 +3827,17 @@
     </row>
     <row r="87" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -4008,17 +3852,17 @@
     </row>
     <row r="88" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -4033,10 +3877,10 @@
     </row>
     <row r="89" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -4055,17 +3899,17 @@
     </row>
     <row r="90" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -4080,17 +3924,17 @@
     </row>
     <row r="91" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -4105,10 +3949,10 @@
     </row>
     <row r="92" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -4127,17 +3971,17 @@
     </row>
     <row r="93" customFormat="false" ht="75.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -4152,17 +3996,17 @@
     </row>
     <row r="94" customFormat="false" ht="138.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -4176,11 +4020,9 @@
       <c r="M94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="19" t="s">
-        <v>264</v>
-      </c>
+      <c r="A95" s="16"/>
       <c r="B95" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -4196,10 +4038,10 @@
     </row>
     <row r="96" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -4218,17 +4060,17 @@
     </row>
     <row r="97" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -4243,17 +4085,17 @@
     </row>
     <row r="98" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -4268,10 +4110,10 @@
     </row>
     <row r="99" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4290,17 +4132,17 @@
     </row>
     <row r="100" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -4315,17 +4157,17 @@
     </row>
     <row r="101" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -4340,10 +4182,10 @@
     </row>
     <row r="102" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -4360,44 +4202,44 @@
       <c r="L102" s="3"/>
       <c r="M102" s="7"/>
     </row>
-    <row r="103" s="16" customFormat="true" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E103" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="14"/>
-      <c r="L103" s="14"/>
-      <c r="M103" s="15"/>
+    <row r="103" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -4412,10 +4254,10 @@
     </row>
     <row r="105" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4434,17 +4276,17 @@
     </row>
     <row r="106" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -4459,17 +4301,17 @@
     </row>
     <row r="107" customFormat="false" ht="157.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -4484,10 +4326,10 @@
     </row>
     <row r="108" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -4506,17 +4348,17 @@
     </row>
     <row r="109" customFormat="false" ht="169.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -4531,17 +4373,17 @@
     </row>
     <row r="110" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -4556,10 +4398,10 @@
     </row>
     <row r="111" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4578,17 +4420,17 @@
     </row>
     <row r="112" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -4603,17 +4445,17 @@
     </row>
     <row r="113" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -4628,10 +4470,10 @@
     </row>
     <row r="114" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4649,18 +4491,18 @@
       <c r="M114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="14" t="s">
-        <v>316</v>
+      <c r="A115" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
@@ -4674,18 +4516,18 @@
       <c r="M115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C116" s="14"/>
+      <c r="A116" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
@@ -4700,10 +4542,10 @@
     </row>
     <row r="117" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -4722,17 +4564,17 @@
     </row>
     <row r="118" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -4747,17 +4589,17 @@
     </row>
     <row r="119" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -4772,10 +4614,10 @@
     </row>
     <row r="120" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -4794,17 +4636,17 @@
     </row>
     <row r="121" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -4819,17 +4661,17 @@
     </row>
     <row r="122" customFormat="false" ht="123" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -4844,10 +4686,10 @@
     </row>
     <row r="123" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -4864,44 +4706,44 @@
       <c r="L123" s="3"/>
       <c r="M123" s="7"/>
     </row>
-    <row r="124" s="27" customFormat="true" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="25" t="s">
-        <v>341</v>
-      </c>
-      <c r="B124" s="25" t="s">
-        <v>342</v>
-      </c>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E124" s="25" t="s">
-        <v>343</v>
-      </c>
-      <c r="F124" s="25"/>
-      <c r="G124" s="25"/>
-      <c r="H124" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="I124" s="25"/>
-      <c r="J124" s="25"/>
-      <c r="K124" s="25"/>
-      <c r="L124" s="25"/>
-      <c r="M124" s="26"/>
+    <row r="124" s="24" customFormat="true" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B124" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="C124" s="22"/>
+      <c r="D124" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E124" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="F124" s="22"/>
+      <c r="G124" s="22"/>
+      <c r="H124" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" s="22"/>
+      <c r="J124" s="22"/>
+      <c r="K124" s="22"/>
+      <c r="L124" s="22"/>
+      <c r="M124" s="23"/>
     </row>
     <row r="125" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -4915,11 +4757,9 @@
       <c r="M125" s="8"/>
     </row>
     <row r="126" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="s">
-        <v>347</v>
-      </c>
+      <c r="A126" s="2"/>
       <c r="B126" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -4935,10 +4775,10 @@
     </row>
     <row r="127" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -4957,17 +4797,17 @@
     </row>
     <row r="128" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C128" s="3"/>
       <c r="D128" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
@@ -4982,17 +4822,17 @@
     </row>
     <row r="129" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -5007,10 +4847,10 @@
     </row>
     <row r="130" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -5029,20 +4869,20 @@
     </row>
     <row r="131" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="E131" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
+        <v>356</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
       <c r="H131" s="8" t="n">
         <v>1</v>
       </c>
@@ -5054,17 +4894,17 @@
     </row>
     <row r="132" customFormat="false" ht="75.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
@@ -5079,10 +4919,10 @@
     </row>
     <row r="133" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -5101,20 +4941,20 @@
     </row>
     <row r="134" customFormat="false" ht="183" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E134" s="28" t="s">
-        <v>370</v>
-      </c>
-      <c r="F134" s="28"/>
-      <c r="G134" s="28"/>
+        <v>11</v>
+      </c>
+      <c r="E134" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
       <c r="H134" s="8" t="n">
         <v>1</v>
       </c>
@@ -5126,17 +4966,17 @@
     </row>
     <row r="135" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="C135" s="14"/>
+        <v>366</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
@@ -5151,10 +4991,10 @@
     </row>
     <row r="136" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -5173,17 +5013,17 @@
     </row>
     <row r="137" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -5198,17 +5038,17 @@
     </row>
     <row r="138" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -5223,10 +5063,10 @@
     </row>
     <row r="139" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -5245,17 +5085,17 @@
     </row>
     <row r="140" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
@@ -5270,17 +5110,17 @@
     </row>
     <row r="141" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -5294,11 +5134,9 @@
       <c r="M141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2" t="s">
-        <v>391</v>
-      </c>
+      <c r="A142" s="2"/>
       <c r="B142" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -5314,10 +5152,10 @@
     </row>
     <row r="143" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -5336,17 +5174,17 @@
     </row>
     <row r="144" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
@@ -5361,17 +5199,17 @@
     </row>
     <row r="145" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="B145" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="C145" s="14"/>
+        <v>393</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -5386,10 +5224,10 @@
     </row>
     <row r="146" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -5408,17 +5246,17 @@
     </row>
     <row r="147" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
@@ -5433,17 +5271,17 @@
     </row>
     <row r="148" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
@@ -5458,10 +5296,10 @@
     </row>
     <row r="149" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -5480,17 +5318,17 @@
     </row>
     <row r="150" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>
@@ -5505,17 +5343,17 @@
     </row>
     <row r="151" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
@@ -5530,10 +5368,10 @@
     </row>
     <row r="152" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -5552,17 +5390,17 @@
     </row>
     <row r="153" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -5577,17 +5415,17 @@
     </row>
     <row r="154" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -5602,10 +5440,10 @@
     </row>
     <row r="155" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -5624,17 +5462,17 @@
     </row>
     <row r="156" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
@@ -5649,17 +5487,17 @@
     </row>
     <row r="157" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -5672,29 +5510,7 @@
       <c r="L157" s="3"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" s="16" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="B158" s="30"/>
-      <c r="C158" s="29"/>
-      <c r="D158" s="29"/>
-      <c r="E158" s="29"/>
-    </row>
-    <row r="159" s="16" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="B159" s="30"/>
-      <c r="C159" s="29"/>
-      <c r="D159" s="29"/>
-      <c r="E159" s="29"/>
-    </row>
-    <row r="160" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="258">
     <mergeCell ref="B1:C1"/>
@@ -6002,7 +5818,7 @@
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H68 H70:H160" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H68 H70:H157" type="list">
       <formula1>$A$158:$A$160</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6018,6 +5834,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>